<commit_message>
automation tests for PAS-12872-verifying the vin refresh on various scenarios
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_CA_CHOICE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Desktop\SUITE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732" tabRatio="384"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,42 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Petrenko, Viktor (C)</author>
-  </authors>
-  <commentList>
-    <comment ref="AA2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Petrenko, Viktor (C):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-User for MSRP PAS-730</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>VIN</t>
   </si>
@@ -144,27 +110,15 @@
     <t>ALTFUEL</t>
   </si>
   <si>
-    <t>WAG</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
-    <t>000R</t>
-  </si>
-  <si>
-    <t>DUAL AIR BAGS FRONT</t>
-  </si>
-  <si>
     <t>4 WHEEL STANDARD</t>
   </si>
   <si>
     <t>STD</t>
   </si>
   <si>
-    <t>B-IMMOBILIZER/KEYLSS ENTRY/ALARM</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -201,31 +155,52 @@
     <t>CHOICE_TIER</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>8L V12</t>
-  </si>
-  <si>
-    <t>4WD</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN</t>
-  </si>
-  <si>
-    <t>GOLF</t>
-  </si>
-  <si>
-    <t>HATCHBACK 4 DOOR</t>
-  </si>
-  <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>7MSRP15H&amp;V</t>
+    <t>1.6L L4</t>
+  </si>
+  <si>
+    <t>2WD</t>
+  </si>
+  <si>
+    <t>1N4BL3AP&amp;H</t>
+  </si>
+  <si>
+    <t>NISS</t>
+  </si>
+  <si>
+    <t>SED</t>
+  </si>
+  <si>
+    <t>DUAL FRNT/HEAD/SIDE/REAR SIDE AIRBAGS</t>
+  </si>
+  <si>
+    <t>F-IMMOBILIZER/KEYLESS ENTRY</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>NISSAN MOTOR</t>
+  </si>
+  <si>
+    <t>NISS ALTIMA</t>
+  </si>
+  <si>
+    <t>ALTIMA 4.5SL</t>
+  </si>
+  <si>
+    <t>NISSAN</t>
+  </si>
+  <si>
+    <t>ALTIMA</t>
+  </si>
+  <si>
+    <t>ALTIMA 3.5SL</t>
+  </si>
+  <si>
+    <t>SEDAN</t>
   </si>
   <si>
     <t>SYMBOL_2000_CHOICE</t>
@@ -235,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,25 +231,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -303,15 +259,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -593,38 +546,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="21" max="21" width="22.85546875" customWidth="1"/>
-    <col min="23" max="23" width="22.28515625" customWidth="1"/>
-    <col min="24" max="24" width="20.85546875" customWidth="1"/>
-    <col min="25" max="25" width="34.7109375" customWidth="1"/>
-    <col min="26" max="26" width="6.5703125" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="29" width="16.28515625" customWidth="1"/>
-    <col min="35" max="35" width="15.140625" customWidth="1"/>
-    <col min="37" max="37" width="22.7109375" customWidth="1"/>
-    <col min="38" max="38" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" customWidth="1"/>
+    <col min="24" max="24" width="20.88671875" customWidth="1"/>
+    <col min="25" max="25" width="34.6640625" customWidth="1"/>
+    <col min="26" max="26" width="6.5546875" customWidth="1"/>
+    <col min="27" max="27" width="14.88671875" customWidth="1"/>
+    <col min="28" max="29" width="16.33203125" customWidth="1"/>
+    <col min="35" max="35" width="15.109375" customWidth="1"/>
+    <col min="37" max="37" width="22.6640625" customWidth="1"/>
+    <col min="38" max="38" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +655,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>25</v>
@@ -710,158 +664,246 @@
         <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H2" s="3">
         <v>88888</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="3">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="3">
-        <v>12</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="Q2" s="3">
         <v>214</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="S2" s="3">
-        <v>4</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="T2" s="3">
+        <v>7</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="V2" s="3">
         <v>2</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AA2" s="3">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="AB2" s="3">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AI2">
         <v>20000101</v>
       </c>
       <c r="AJ2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="3">
+        <v>88888</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="3">
+        <v>6</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>214</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+      <c r="S3" s="3">
+        <v>2</v>
+      </c>
+      <c r="T3" s="3">
+        <v>7</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" s="3">
+        <v>2</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI3">
+        <v>20180612</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>